<commit_message>
Separate movies to be added in two different sheets.
</commit_message>
<xml_diff>
--- a/database.xlsx
+++ b/database.xlsx
@@ -7,6 +7,7 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Recommended" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="162913" fullCalcOnLoad="1"/>
@@ -390,7 +391,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A6"/>
+  <dimension ref="A1:A8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -440,7 +441,75 @@
         </is>
       </c>
     </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>We are The Millers</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Into The Wild</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Indiana Jones</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Catch Me If You Can</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Titanic</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>The Prestige</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Titanic</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>